<commit_message>
Adding labels to stats and commenting code
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0678210d0a0b8db/Ambiente de Trabalho/ia_t1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_B7778A11B63BB3D9D4B19471090DA9EE5EAB9AF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67B23B91-DF92-45DC-93EC-528127AA4B3D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Execution Time" sheetId="1" r:id="rId1"/>
     <sheet name="Memory Usage" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>depth</t>
   </si>
@@ -76,12 +70,15 @@
   <si>
     <t>Maze 5</t>
   </si>
+  <si>
+    <t>Maze 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,37 +141,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -194,9 +171,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -211,40 +188,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$B$2:$B$6</c:f>
+              <c:f>'Execution Time'!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.4531373977661129E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.1253776550292969E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3280630111694339E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1082699298858643</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.9258213043212891E-3</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.01716232299804688</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.008615255355834961</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01722025871276855</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1443655490875244</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.009601831436157227</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1166551113128662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -265,9 +242,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -282,40 +259,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$C$2:$C$6</c:f>
+              <c:f>'Execution Time'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>3.1523704528808587E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6091823577880859E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9050836563110352E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.2557907104492188E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.5314979553222656E-3</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.06823015213012695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01758646965026855</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02474069595336914</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0829617977142334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01206302642822266</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.08032369613647461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -336,9 +313,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -353,40 +330,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$D$2:$D$6</c:f>
+              <c:f>'Execution Time'!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5.9856891632080078E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.5834732055664063E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.5394430160522461E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0001659393310549E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1070966720581049E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.07553768157958984</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01164674758911133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04384517669677734</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.002022266387939453</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01460742950439453</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00101161003112793</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -407,9 +384,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -424,40 +401,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$E$2:$E$6</c:f>
+              <c:f>'Execution Time'!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>7.1593523025512695E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.6578426361083981E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.106784820556641E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0242671966552726E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5385866165161129E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.09587621688842773</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03079724311828613</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03778553009033203</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.004983901977539062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01792645454406738</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.005597114562988281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -478,9 +455,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -495,40 +472,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$F$2:$F$6</c:f>
+              <c:f>'Execution Time'!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6.6287040710449219E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.45518684387207E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0665397644042969E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.9977092742919922E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5052080154418951E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0826716423034668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02837252616882324</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03920149803161621</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.003007888793945312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01811051368713379</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.003007888793945312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -549,9 +526,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -566,40 +543,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$G$2:$G$6</c:f>
+              <c:f>'Execution Time'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>7.0326566696166992E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0090341567993161E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.9586305618286133E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0170211791992192E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4539957046508791E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.09094977378845215</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02524566650390625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04629683494567871</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.003209829330444336</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01654863357543945</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00255131721496582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -620,9 +597,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -637,40 +614,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$H$2:$H$6</c:f>
+              <c:f>'Execution Time'!$H$2:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9.8938226699829102E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.762556076049805E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.4873485565185547E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.31370806694030762</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.3517856597900391E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1165740489959717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.04194283485412598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04500627517700195</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.389542818069458</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01713347434997559</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3804805278778076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -691,9 +668,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -708,40 +685,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$I$2:$I$6</c:f>
+              <c:f>'Execution Time'!$I$2:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9.2776298522949219E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.959847450256348E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.7579536437988281E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.1301441192626953E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5090227127075201E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1080152988433838</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03485202789306641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04234027862548828</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1783123016357422</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01990604400634766</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1158096790313721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
@@ -762,9 +739,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -779,40 +756,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$J$2:$J$6</c:f>
+              <c:f>'Execution Time'!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>7.1217060089111328E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.8058538436889648E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.5629978179931641E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4920234680175779E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.0047903060913089E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.09156632423400879</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02164721488952637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05687499046325684</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.003012418746948242</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02410101890563965</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0035247802734375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
@@ -833,9 +810,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -850,40 +827,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$K$2:$K$6</c:f>
+              <c:f>'Execution Time'!$K$2:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.10009264945983889</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.7761936187744141E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.8610219955444343E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2321324348449707</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.503276824951172E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1220412254333496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03421521186828613</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04593586921691895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2831780910491943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01981711387634277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3034822940826416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
@@ -904,9 +881,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -921,40 +898,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$L$2:$L$6</c:f>
+              <c:f>'Execution Time'!$L$2:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9.5781087875366211E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.8076887130737301E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.8617134094238281E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.2377462387084961E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6058683395385739E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1382465362548828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03977847099304199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05380964279174805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06877613067626953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02460837364196777</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.07208609580993652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
@@ -975,9 +952,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -992,40 +969,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$M$2:$M$6</c:f>
+              <c:f>'Execution Time'!$M$2:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9849700927734375E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5063285827636721E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.001999616622924805</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0005078315734863281</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001006603240966797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0009996891021728516</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.001013040542602539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="12"/>
@@ -1046,9 +1023,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Execution Time'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Execution Time'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1063,50 +1040,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Time'!$N$2:$N$6</c:f>
+              <c:f>'Execution Time'!$N$2:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>3.4116029739379883E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.453018188476562E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6844272613525391E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.4660787582397461E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.5289478302001953E-3</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.02159595489501953</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01514029502868652</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0175011157989502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1978034973144531</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01056599617004395</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1057941913604736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-D407-4627-A0E0-26FD3E045B17}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
+        <c:marker val="1"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
       </c:lineChart>
@@ -1115,30 +1084,58 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mazes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
@@ -1147,11 +1144,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1162,25 +1157,13 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1200,9 +1183,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1217,16 +1200,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$B$2:$B$6</c:f>
+              <c:f>'Memory Usage'!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>229255</c:v>
                 </c:pt>
@@ -1241,16 +1227,13 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>56296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2301104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1271,9 +1254,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1288,40 +1271,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$C$2:$C$6</c:f>
+              <c:f>'Memory Usage'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>749464</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>292448</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>402408</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1970520</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>161880</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>749768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>292504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>392808</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1979872</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>161824</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1963992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1342,9 +1325,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1359,40 +1342,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$D$2:$D$6</c:f>
+              <c:f>'Memory Usage'!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>188697</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>46632</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>144395</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>187537</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46608</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144371</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13624</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>58600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1413,9 +1396,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1430,18 +1413,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$E$2:$E$6</c:f>
+              <c:f>'Memory Usage'!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>189456</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>194232</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>81115</c:v>
@@ -1450,20 +1436,17 @@
                   <c:v>132496</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41488</c:v>
+                  <c:v>41056</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>55160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40792</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1484,9 +1467,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1501,18 +1484,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$F$2:$F$6</c:f>
+              <c:f>'Memory Usage'!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>180040</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>182384</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>74096</c:v>
@@ -1525,16 +1511,13 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>58816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1555,9 +1538,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1572,18 +1555,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$G$2:$G$6</c:f>
+              <c:f>'Memory Usage'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>208794</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>192978</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70080</c:v>
@@ -1596,16 +1582,13 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>61560</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -1626,9 +1609,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1643,18 +1626,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$H$2:$H$6</c:f>
+              <c:f>'Memory Usage'!$H$2:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>213568</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>208408</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>103296</c:v>
@@ -1663,20 +1649,17 @@
                   <c:v>126448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>376752</c:v>
+                  <c:v>376800</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>54504</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>376680</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -1697,9 +1680,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1714,18 +1697,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$I$2:$I$6</c:f>
+              <c:f>'Memory Usage'!$I$2:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>200688</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>194368</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>79128</c:v>
@@ -1734,20 +1720,17 @@
                   <c:v>132216</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>204160</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>63496</c:v>
+                  <c:v>205184</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63552</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>204136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
@@ -1768,9 +1751,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1785,18 +1768,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$J$2:$J$6</c:f>
+              <c:f>'Memory Usage'!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>178872</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>182320</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>65944</c:v>
@@ -1809,16 +1795,13 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>67244</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
@@ -1839,9 +1822,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1856,18 +1839,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$K$2:$K$6</c:f>
+              <c:f>'Memory Usage'!$K$2:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>199564</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>199356</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>104000</c:v>
@@ -1880,16 +1866,13 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>55448</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>334040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
@@ -1910,9 +1893,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1927,18 +1910,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$L$2:$L$6</c:f>
+              <c:f>'Memory Usage'!$L$2:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>192508</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>190228</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>78880</c:v>
@@ -1951,16 +1937,13 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>62000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
@@ -1981,9 +1964,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -1998,16 +1981,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$M$2:$M$6</c:f>
+              <c:f>'Memory Usage'!$M$2:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1360</c:v>
                 </c:pt>
@@ -2021,17 +2007,14 @@
                   <c:v>336</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="12"/>
@@ -2052,9 +2035,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Memory Usage'!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>'Memory Usage'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Maze 1</c:v>
                 </c:pt>
@@ -2069,50 +2052,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Maze 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Maze 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Memory Usage'!$N$2:$N$6</c:f>
+              <c:f>'Memory Usage'!$N$2:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>299336</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>87712</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>147774</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1524876</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>59712</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>272288</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108472</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2613402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67616</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1904800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-3AC6-464B-B793-2E614EA75EB2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
+        <c:marker val="1"/>
         <c:axId val="50020001"/>
         <c:axId val="50020002"/>
       </c:lineChart>
@@ -2121,30 +2096,58 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mazes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50020002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
@@ -2153,11 +2156,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2171,26 +2172,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2212,26 +2207,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2292,7 +2281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2324,27 +2313,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2376,24 +2347,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2569,16 +2522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2619,224 +2570,268 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>1.4531373977661129E-2</v>
+        <v>0.01716232299804688</v>
       </c>
       <c r="C2">
-        <v>3.1523704528808587E-2</v>
+        <v>0.06823015213012695</v>
       </c>
       <c r="D2">
-        <v>5.9856891632080078E-2</v>
+        <v>0.07553768157958984</v>
       </c>
       <c r="E2">
-        <v>7.1593523025512695E-2</v>
+        <v>0.09587621688842773</v>
       </c>
       <c r="F2">
-        <v>6.6287040710449219E-2</v>
+        <v>0.0826716423034668</v>
       </c>
       <c r="G2">
-        <v>7.0326566696166992E-2</v>
+        <v>0.09094977378845215</v>
       </c>
       <c r="H2">
-        <v>9.8938226699829102E-2</v>
+        <v>0.1165740489959717</v>
       </c>
       <c r="I2">
-        <v>9.2776298522949219E-2</v>
+        <v>0.1080152988433838</v>
       </c>
       <c r="J2">
-        <v>7.1217060089111328E-2</v>
+        <v>0.09156632423400879</v>
       </c>
       <c r="K2">
-        <v>0.10009264945983889</v>
+        <v>0.1220412254333496</v>
       </c>
       <c r="L2">
-        <v>9.5781087875366211E-2</v>
+        <v>0.1382465362548828</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>3.4116029739379883E-2</v>
+        <v>0.02159595489501953</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>7.1253776550292969E-3</v>
+        <v>0.008615255355834961</v>
       </c>
       <c r="C3">
-        <v>1.6091823577880859E-2</v>
+        <v>0.01758646965026855</v>
       </c>
       <c r="D3">
-        <v>9.5834732055664063E-3</v>
+        <v>0.01164674758911133</v>
       </c>
       <c r="E3">
-        <v>2.6578426361083981E-2</v>
+        <v>0.03079724311828613</v>
       </c>
       <c r="F3">
-        <v>2.45518684387207E-2</v>
+        <v>0.02837252616882324</v>
       </c>
       <c r="G3">
-        <v>2.0090341567993161E-2</v>
+        <v>0.02524566650390625</v>
       </c>
       <c r="H3">
-        <v>2.762556076049805E-2</v>
+        <v>0.04194283485412598</v>
       </c>
       <c r="I3">
-        <v>2.959847450256348E-2</v>
+        <v>0.03485202789306641</v>
       </c>
       <c r="J3">
-        <v>1.8058538436889648E-2</v>
+        <v>0.02164721488952637</v>
       </c>
       <c r="K3">
-        <v>2.7761936187744141E-2</v>
+        <v>0.03421521186828613</v>
       </c>
       <c r="L3">
-        <v>2.8076887130737301E-2</v>
+        <v>0.03977847099304199</v>
       </c>
       <c r="M3">
-        <v>9.9849700927734375E-4</v>
+        <v>0.001999616622924805</v>
       </c>
       <c r="N3">
-        <v>1.453018188476562E-2</v>
+        <v>0.01514029502868652</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>1.3280630111694339E-2</v>
+        <v>0.01722025871276855</v>
       </c>
       <c r="C4">
-        <v>1.9050836563110352E-2</v>
+        <v>0.02474069595336914</v>
       </c>
       <c r="D4">
-        <v>3.5394430160522461E-2</v>
+        <v>0.04384517669677734</v>
       </c>
       <c r="E4">
-        <v>3.106784820556641E-2</v>
+        <v>0.03778553009033203</v>
       </c>
       <c r="F4">
-        <v>3.0665397644042969E-2</v>
+        <v>0.03920149803161621</v>
       </c>
       <c r="G4">
-        <v>3.9586305618286133E-2</v>
+        <v>0.04629683494567871</v>
       </c>
       <c r="H4">
-        <v>3.4873485565185547E-2</v>
+        <v>0.04500627517700195</v>
       </c>
       <c r="I4">
-        <v>3.7579536437988281E-2</v>
+        <v>0.04234027862548828</v>
       </c>
       <c r="J4">
-        <v>4.5629978179931641E-2</v>
+        <v>0.05687499046325684</v>
       </c>
       <c r="K4">
-        <v>3.8610219955444343E-2</v>
+        <v>0.04593586921691895</v>
       </c>
       <c r="L4">
-        <v>3.8617134094238281E-2</v>
+        <v>0.05380964279174805</v>
       </c>
       <c r="M4">
-        <v>1.5063285827636721E-3</v>
+        <v>0.0005078315734863281</v>
       </c>
       <c r="N4">
-        <v>1.6844272613525391E-2</v>
+        <v>0.0175011157989502</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.1082699298858643</v>
+        <v>0.1443655490875244</v>
       </c>
       <c r="C5">
-        <v>9.2557907104492188E-2</v>
+        <v>0.0829617977142334</v>
       </c>
       <c r="D5">
-        <v>1.0001659393310549E-3</v>
+        <v>0.002022266387939453</v>
       </c>
       <c r="E5">
-        <v>4.0242671966552726E-3</v>
+        <v>0.004983901977539062</v>
       </c>
       <c r="F5">
-        <v>1.9977092742919922E-3</v>
+        <v>0.003007888793945312</v>
       </c>
       <c r="G5">
-        <v>2.0170211791992192E-3</v>
+        <v>0.003209829330444336</v>
       </c>
       <c r="H5">
-        <v>0.31370806694030762</v>
+        <v>0.389542818069458</v>
       </c>
       <c r="I5">
-        <v>9.1301441192626953E-2</v>
+        <v>0.1783123016357422</v>
       </c>
       <c r="J5">
-        <v>1.4920234680175779E-3</v>
+        <v>0.003012418746948242</v>
       </c>
       <c r="K5">
-        <v>0.2321324348449707</v>
+        <v>0.2831780910491943</v>
       </c>
       <c r="L5">
-        <v>5.2377462387084961E-2</v>
+        <v>0.06877613067626953</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>0.001006603240966797</v>
       </c>
       <c r="N5">
-        <v>6.4660787582397461E-2</v>
+        <v>0.1978034973144531</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>6.9258213043212891E-3</v>
+        <v>0.009601831436157227</v>
       </c>
       <c r="C6">
-        <v>9.5314979553222656E-3</v>
+        <v>0.01206302642822266</v>
       </c>
       <c r="D6">
-        <v>1.1070966720581049E-2</v>
+        <v>0.01460742950439453</v>
       </c>
       <c r="E6">
-        <v>1.5385866165161129E-2</v>
+        <v>0.01792645454406738</v>
       </c>
       <c r="F6">
-        <v>1.5052080154418951E-2</v>
+        <v>0.01811051368713379</v>
       </c>
       <c r="G6">
-        <v>1.4539957046508791E-2</v>
+        <v>0.01654863357543945</v>
       </c>
       <c r="H6">
-        <v>1.3517856597900391E-2</v>
+        <v>0.01713347434997559</v>
       </c>
       <c r="I6">
-        <v>1.5090227127075201E-2</v>
+        <v>0.01990604400634766</v>
       </c>
       <c r="J6">
-        <v>2.0047903060913089E-2</v>
+        <v>0.02410101890563965</v>
       </c>
       <c r="K6">
-        <v>1.503276824951172E-2</v>
+        <v>0.01981711387634277</v>
       </c>
       <c r="L6">
-        <v>1.6058683395385739E-2</v>
+        <v>0.02460837364196777</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>0.0009996891021728516</v>
       </c>
       <c r="N6">
-        <v>8.5289478302001953E-3</v>
+        <v>0.01056599617004395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>0.1166551113128662</v>
+      </c>
+      <c r="C7">
+        <v>0.08032369613647461</v>
+      </c>
+      <c r="D7">
+        <v>0.00101161003112793</v>
+      </c>
+      <c r="E7">
+        <v>0.005597114562988281</v>
+      </c>
+      <c r="F7">
+        <v>0.003007888793945312</v>
+      </c>
+      <c r="G7">
+        <v>0.00255131721496582</v>
+      </c>
+      <c r="H7">
+        <v>0.3804805278778076</v>
+      </c>
+      <c r="I7">
+        <v>0.1158096790313721</v>
+      </c>
+      <c r="J7">
+        <v>0.0035247802734375</v>
+      </c>
+      <c r="K7">
+        <v>0.3034822940826416</v>
+      </c>
+      <c r="L7">
+        <v>0.07208609580993652</v>
+      </c>
+      <c r="M7">
+        <v>0.001013040542602539</v>
+      </c>
+      <c r="N7">
+        <v>0.1057941913604736</v>
       </c>
     </row>
   </sheetData>
@@ -2846,16 +2841,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2896,7 +2889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -2904,43 +2897,43 @@
         <v>229255</v>
       </c>
       <c r="C2">
-        <v>749464</v>
+        <v>749768</v>
       </c>
       <c r="D2">
-        <v>188697</v>
+        <v>187537</v>
       </c>
       <c r="E2">
-        <v>189456</v>
+        <v>194232</v>
       </c>
       <c r="F2">
-        <v>180040</v>
+        <v>182384</v>
       </c>
       <c r="G2">
-        <v>208794</v>
+        <v>192978</v>
       </c>
       <c r="H2">
-        <v>213568</v>
+        <v>208408</v>
       </c>
       <c r="I2">
-        <v>200688</v>
+        <v>194368</v>
       </c>
       <c r="J2">
-        <v>178872</v>
+        <v>182320</v>
       </c>
       <c r="K2">
-        <v>199564</v>
+        <v>199356</v>
       </c>
       <c r="L2">
-        <v>192508</v>
+        <v>190228</v>
       </c>
       <c r="M2">
         <v>1360</v>
       </c>
       <c r="N2">
-        <v>299336</v>
+        <v>272288</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2948,10 +2941,10 @@
         <v>50564</v>
       </c>
       <c r="C3">
-        <v>292448</v>
+        <v>292504</v>
       </c>
       <c r="D3">
-        <v>46632</v>
+        <v>46608</v>
       </c>
       <c r="E3">
         <v>81115</v>
@@ -2981,10 +2974,10 @@
         <v>336</v>
       </c>
       <c r="N3">
-        <v>87712</v>
+        <v>79168</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2992,10 +2985,10 @@
         <v>159176</v>
       </c>
       <c r="C4">
-        <v>402408</v>
+        <v>392808</v>
       </c>
       <c r="D4">
-        <v>144395</v>
+        <v>144371</v>
       </c>
       <c r="E4">
         <v>132496</v>
@@ -3025,10 +3018,10 @@
         <v>336</v>
       </c>
       <c r="N4">
-        <v>147774</v>
+        <v>108472</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3036,13 +3029,13 @@
         <v>2301980</v>
       </c>
       <c r="C5">
-        <v>1970520</v>
+        <v>1979872</v>
       </c>
       <c r="D5">
         <v>13624</v>
       </c>
       <c r="E5">
-        <v>41488</v>
+        <v>41056</v>
       </c>
       <c r="F5">
         <v>21696</v>
@@ -3051,10 +3044,10 @@
         <v>18600</v>
       </c>
       <c r="H5">
-        <v>376752</v>
+        <v>376800</v>
       </c>
       <c r="I5">
-        <v>204160</v>
+        <v>205184</v>
       </c>
       <c r="J5">
         <v>18296</v>
@@ -3069,10 +3062,10 @@
         <v>336</v>
       </c>
       <c r="N5">
-        <v>1524876</v>
+        <v>2613402</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -3080,7 +3073,7 @@
         <v>56296</v>
       </c>
       <c r="C6">
-        <v>161880</v>
+        <v>161824</v>
       </c>
       <c r="D6">
         <v>58600</v>
@@ -3098,7 +3091,7 @@
         <v>54504</v>
       </c>
       <c r="I6">
-        <v>63496</v>
+        <v>63552</v>
       </c>
       <c r="J6">
         <v>67244</v>
@@ -3113,7 +3106,51 @@
         <v>336</v>
       </c>
       <c r="N6">
-        <v>59712</v>
+        <v>67616</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>2301104</v>
+      </c>
+      <c r="C7">
+        <v>1963992</v>
+      </c>
+      <c r="D7">
+        <v>13624</v>
+      </c>
+      <c r="E7">
+        <v>40792</v>
+      </c>
+      <c r="F7">
+        <v>21696</v>
+      </c>
+      <c r="G7">
+        <v>18600</v>
+      </c>
+      <c r="H7">
+        <v>376680</v>
+      </c>
+      <c r="I7">
+        <v>204136</v>
+      </c>
+      <c r="J7">
+        <v>18296</v>
+      </c>
+      <c r="K7">
+        <v>334040</v>
+      </c>
+      <c r="L7">
+        <v>162248</v>
+      </c>
+      <c r="M7">
+        <v>336</v>
+      </c>
+      <c r="N7">
+        <v>1904800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>